<commit_message>
added tab for retrospective data dictionary
</commit_message>
<xml_diff>
--- a/gearss_data_dictionary_wOMOP.xlsx
+++ b/gearss_data_dictionary_wOMOP.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dm2569/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D8A104-5FDF-D240-BADB-2E8D371FA4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4625E2B9-2519-CC4B-8B23-1E00BE7A3AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3820" yWindow="1600" windowWidth="25240" windowHeight="13940" activeTab="1" xr2:uid="{322A892C-5887-4F4F-8F63-E3A9ECA846B3}"/>
+    <workbookView xWindow="3820" yWindow="1600" windowWidth="25240" windowHeight="17380" activeTab="1" xr2:uid="{322A892C-5887-4F4F-8F63-E3A9ECA846B3}"/>
   </bookViews>
   <sheets>
-    <sheet name="gearss_data_dictionary_wOMOP" sheetId="1" r:id="rId1"/>
-    <sheet name="notes" sheetId="2" r:id="rId2"/>
-    <sheet name="QUERY SPECIFICATIONS" sheetId="3" r:id="rId3"/>
+    <sheet name="PROSPECTIVE" sheetId="1" r:id="rId1"/>
+    <sheet name="RETROSPECTIVE" sheetId="4" r:id="rId2"/>
+    <sheet name="notes" sheetId="2" r:id="rId3"/>
+    <sheet name="QUERY SPECIFICATIONS" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gearss_data_dictionary_wOMOP!$A$1:$F$764</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PROSPECTIVE!$A$1:$F$764</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -4631,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F1CBD9-DAA2-4C41-BF28-1B48A61D2B7C}">
   <dimension ref="A1:H764"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19473,11 +19487,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE8CC84-DA5A-5D47-A279-16EBF4A1F059}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441977DD-205E-AB4D-BCFC-B1037F480A58}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -19565,7 +19593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1674E32-5A9E-A54C-A930-4C89C7A8984A}">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>